<commit_message>
Refactered the playwright into BDD cucmber pattern
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/LoginTestData.xlsx
+++ b/src/test/resources/testdata/LoginTestData.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nelson_Personal\IdeaProjects\Pact-lab\playwright_repo\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF7AAA3C-290F-49E3-A046-11EBEFF3AC0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C34215A4-5FED-444A-A22B-BC2DB654D70F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-80" yWindow="-80" windowWidth="19360" windowHeight="11440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginData" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>username</t>
   </si>
@@ -40,6 +41,9 @@
   </si>
   <si>
     <t>Password124</t>
+  </si>
+  <si>
+    <t>studentexcel</t>
   </si>
 </sst>
 </file>
@@ -366,7 +370,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -385,7 +389,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>

</xml_diff>